<commit_message>
First push to repo
</commit_message>
<xml_diff>
--- a/Loantape.xlsx
+++ b/Loantape.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ljurkowski001\PycharmProjects\VWcomparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2FB4F76-9DE3-4341-AFA6-D02B0695332C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{624E07BB-4620-4185-96EB-A46FD5FF40DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,7 +631,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>